<commit_message>
Just tweaks in diagnostictelemetry and the matching spreadsheet.
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecGolf-T.xlsx
+++ b/genSpacecraft/DownlinkSpecGolf-T.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2190" uniqueCount="632">
   <si>
     <t xml:space="preserve">//</t>
   </si>
@@ -1283,49 +1283,49 @@
     <t xml:space="preserve">Legacy  Errors</t>
   </si>
   <si>
-    <t xml:space="preserve">Tasks that have reported to watchdog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">legWdReports</t>
+    <t xml:space="preserve">LIHU: WDTasks Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LegWdReports</t>
   </si>
   <si>
     <t xml:space="preserve">IHU Reset Info</t>
   </si>
   <si>
-    <t xml:space="preserve">Error that caused the last reset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">legErrorCode</t>
+    <t xml:space="preserve">Cause of Reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LegErrorCode</t>
   </si>
   <si>
     <t xml:space="preserve">Task executing at reset</t>
   </si>
   <si>
-    <t xml:space="preserve">legTaskNumber</t>
+    <t xml:space="preserve">LegTaskNumber</t>
   </si>
   <si>
     <t xml:space="preserve">Previous task before reset</t>
   </si>
   <si>
-    <t xml:space="preserve">legPreviousTask</t>
+    <t xml:space="preserve">LegPreviousTask</t>
   </si>
   <si>
     <t xml:space="preserve">Resets in a row that have been too soon</t>
   </si>
   <si>
-    <t xml:space="preserve">legEarlyResetCount</t>
+    <t xml:space="preserve">LegEarlyResetCount</t>
   </si>
   <si>
     <t xml:space="preserve">Was this reset still early in boot</t>
   </si>
   <si>
-    <t xml:space="preserve">legWasStillEarlyInBoot</t>
+    <t xml:space="preserve">LegWasStillEarlyInBoot</t>
   </si>
   <si>
     <t xml:space="preserve">LIHU Data Valid</t>
   </si>
   <si>
-    <t xml:space="preserve">legValid</t>
+    <t xml:space="preserve">LegValid</t>
   </si>
   <si>
     <t xml:space="preserve">STATUS_BOOLEAN</t>
@@ -1334,7 +1334,7 @@
     <t xml:space="preserve">pad to 32 bits</t>
   </si>
   <si>
-    <t xml:space="preserve">legFiller1</t>
+    <t xml:space="preserve">LegFiller1</t>
   </si>
   <si>
     <t xml:space="preserve">INT</t>
@@ -1346,7 +1346,7 @@
     <t xml:space="preserve">GOLF_LIHU_ERR</t>
   </si>
   <si>
-    <t xml:space="preserve">LIHU: Tasks That Reported</t>
+    <t xml:space="preserve">LIHU: WD Tasks Ok</t>
   </si>
   <si>
     <t xml:space="preserve">I2C1 Errors</t>
@@ -1391,6 +1391,9 @@
     <t xml:space="preserve">LegMramRead</t>
   </si>
   <si>
+    <t xml:space="preserve">legacy  Errors</t>
+  </si>
+  <si>
     <t xml:space="preserve">MRAM Write Error</t>
   </si>
   <si>
@@ -1418,12 +1421,18 @@
     <t xml:space="preserve">SWVersion</t>
   </si>
   <si>
-    <t xml:space="preserve">pad11</t>
+    <t xml:space="preserve">Error Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LegErrorData</t>
   </si>
   <si>
     <t xml:space="preserve">Structure:rt1Errors_t,file:rt1ErrorsDownlink.h</t>
   </si>
   <si>
+    <t xml:space="preserve">Watchdog Tasks Ok</t>
+  </si>
+  <si>
     <t xml:space="preserve">wdReports</t>
   </si>
   <si>
@@ -1454,24 +1463,21 @@
     <t xml:space="preserve">GOLF_RTIHU_ERR</t>
   </si>
   <si>
-    <t xml:space="preserve">RTIHU1: Tasks That Reported</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data passed to error call that might have caused reset</t>
+    <t xml:space="preserve">RTIHU1: WD Tasks Ok</t>
   </si>
   <si>
     <t xml:space="preserve">errorData</t>
   </si>
   <si>
+    <t xml:space="preserve">Primary SRAM Corrected Addr 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAMCorAddr1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Primary RT Errors</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary SRAM Corrected Addr 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAMCorAddr1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Primary SRAM Corrected Addr 2</t>
   </si>
   <si>
@@ -1658,7 +1664,7 @@
     <t xml:space="preserve">nonFatalCnt</t>
   </si>
   <si>
-    <t xml:space="preserve">Version Number</t>
+    <t xml:space="preserve">RTIHU1 Version Number</t>
   </si>
   <si>
     <t xml:space="preserve">Unisgned</t>
@@ -1667,6 +1673,9 @@
     <t xml:space="preserve">Structure:rt2Errors_t,file:rt2ErrorsDownlink.h</t>
   </si>
   <si>
+    <t xml:space="preserve">RTIHU2: Watchdog Tasks Ok</t>
+  </si>
+  <si>
     <t xml:space="preserve">RT2wdReports</t>
   </si>
   <si>
@@ -1694,9 +1703,6 @@
     <t xml:space="preserve">filler2</t>
   </si>
   <si>
-    <t xml:space="preserve">RTIHU2: Tasks That Reported</t>
-  </si>
-  <si>
     <t xml:space="preserve">Secndry RT Errors</t>
   </si>
   <si>
@@ -1890,6 +1896,9 @@
   </si>
   <si>
     <t xml:space="preserve">RT2NonFatalCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTIHU2 Version Number</t>
   </si>
   <si>
     <t xml:space="preserve">Payloads per Frame</t>
@@ -2257,8 +2266,8 @@
   </sheetPr>
   <dimension ref="A1:Q397"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D269" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N295" activeCellId="0" sqref="N295"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A275" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J361" activeCellId="0" sqref="J361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2268,10 +2277,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="31.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="33.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="37.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="5" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.66"/>
@@ -12929,7 +12938,7 @@
         <v>2</v>
       </c>
       <c r="P258" s="38" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q258" s="38" t="n">
         <v>0</v>
@@ -12981,7 +12990,7 @@
         <v>2</v>
       </c>
       <c r="P259" s="38" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q259" s="38" t="n">
         <v>0</v>
@@ -13033,7 +13042,7 @@
         <v>2</v>
       </c>
       <c r="P260" s="38" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q260" s="38" t="n">
         <v>0</v>
@@ -13085,7 +13094,7 @@
         <v>2</v>
       </c>
       <c r="P261" s="38" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q261" s="38" t="n">
         <v>0</v>
@@ -13565,7 +13574,7 @@
         <v>5.5</v>
       </c>
       <c r="N271" s="1" t="s">
-        <v>419</v>
+        <v>456</v>
       </c>
       <c r="O271" s="1" t="n">
         <v>3</v>
@@ -13579,10 +13588,10 @@
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B272" s="3" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C272" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D272" s="1" t="n">
         <v>8</v>
@@ -13631,10 +13640,10 @@
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B273" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C273" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D273" s="1" t="n">
         <v>8</v>
@@ -13683,10 +13692,10 @@
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B274" s="3" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C274" s="3" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D274" s="1" t="n">
         <v>8</v>
@@ -13735,10 +13744,10 @@
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B275" s="3" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C275" s="3" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D275" s="1" t="n">
         <v>8</v>
@@ -13787,10 +13796,10 @@
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B276" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C276" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D276" s="1" t="n">
         <v>8</v>
@@ -13839,10 +13848,10 @@
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B277" s="3" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D277" s="1" t="n">
         <v>8</v>
@@ -13891,10 +13900,10 @@
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B278" s="3" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C278" s="3" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D278" s="1" t="n">
         <v>16</v>
@@ -13931,10 +13940,10 @@
         <v>7.25</v>
       </c>
       <c r="N278" s="1" t="s">
-        <v>419</v>
+        <v>402</v>
       </c>
       <c r="O278" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P278" s="1" t="n">
         <v>14</v>
@@ -13945,10 +13954,10 @@
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B279" s="3" t="s">
-        <v>417</v>
+        <v>466</v>
       </c>
       <c r="C279" s="3" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="D279" s="1" t="n">
         <v>8</v>
@@ -13957,8 +13966,8 @@
         <v>26</v>
       </c>
       <c r="F279" s="33"/>
-      <c r="G279" s="33" t="n">
-        <v>0</v>
+      <c r="G279" s="33" t="s">
+        <v>438</v>
       </c>
       <c r="H279" s="33" t="s">
         <v>27</v>
@@ -13983,13 +13992,13 @@
         <v>7.75</v>
       </c>
       <c r="N279" s="1" t="s">
-        <v>29</v>
+        <v>422</v>
       </c>
       <c r="O279" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P279" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q279" s="1" t="n">
         <v>0</v>
@@ -14022,7 +14031,7 @@
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="36" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="J281" s="37"/>
       <c r="K281" s="25"/>
@@ -14104,10 +14113,10 @@
     </row>
     <row r="284" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B284" s="21" t="s">
-        <v>420</v>
+        <v>469</v>
       </c>
       <c r="C284" s="39" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="D284" s="1" t="n">
         <v>9</v>
@@ -14159,7 +14168,7 @@
         <v>423</v>
       </c>
       <c r="C285" s="39" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="D285" s="1" t="n">
         <v>5</v>
@@ -14211,7 +14220,7 @@
         <v>425</v>
       </c>
       <c r="C286" s="39" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="D286" s="1" t="n">
         <v>4</v>
@@ -14263,7 +14272,7 @@
         <v>427</v>
       </c>
       <c r="C287" s="39" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="D287" s="1" t="n">
         <v>4</v>
@@ -14315,7 +14324,7 @@
         <v>429</v>
       </c>
       <c r="C288" s="39" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="D288" s="1" t="n">
         <v>3</v>
@@ -14367,7 +14376,7 @@
         <v>431</v>
       </c>
       <c r="C289" s="39" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="D289" s="1" t="n">
         <v>1</v>
@@ -14416,10 +14425,10 @@
     </row>
     <row r="290" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B290" s="21" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="C290" s="39" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="D290" s="1" t="n">
         <v>1</v>
@@ -14471,7 +14480,7 @@
         <v>436</v>
       </c>
       <c r="C291" s="39" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="D291" s="1" t="n">
         <v>5</v>
@@ -14557,7 +14566,7 @@
         <v>436</v>
       </c>
       <c r="C294" s="39" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="D294" s="1" t="n">
         <v>5</v>
@@ -14606,10 +14615,10 @@
     </row>
     <row r="295" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B295" s="21" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="C295" s="39" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="D295" s="1" t="n">
         <v>1</v>
@@ -14661,7 +14670,7 @@
         <v>431</v>
       </c>
       <c r="C296" s="39" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="D296" s="1" t="n">
         <v>1</v>
@@ -14702,7 +14711,7 @@
         <v>2</v>
       </c>
       <c r="P296" s="38" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="Q296" s="38" t="n">
         <v>0</v>
@@ -14713,7 +14722,7 @@
         <v>429</v>
       </c>
       <c r="C297" s="39" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="D297" s="1" t="n">
         <v>3</v>
@@ -14754,7 +14763,7 @@
         <v>2</v>
       </c>
       <c r="P297" s="38" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="Q297" s="38" t="n">
         <v>0</v>
@@ -14765,7 +14774,7 @@
         <v>427</v>
       </c>
       <c r="C298" s="39" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="D298" s="1" t="n">
         <v>4</v>
@@ -14806,7 +14815,7 @@
         <v>2</v>
       </c>
       <c r="P298" s="38" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q298" s="38" t="n">
         <v>0</v>
@@ -14817,7 +14826,7 @@
         <v>425</v>
       </c>
       <c r="C299" s="39" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="D299" s="1" t="n">
         <v>4</v>
@@ -14858,7 +14867,7 @@
         <v>2</v>
       </c>
       <c r="P299" s="38" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="Q299" s="38" t="n">
         <v>0</v>
@@ -14869,7 +14878,7 @@
         <v>423</v>
       </c>
       <c r="C300" s="39" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="D300" s="1" t="n">
         <v>5</v>
@@ -14879,7 +14888,7 @@
       </c>
       <c r="F300" s="40"/>
       <c r="G300" s="33" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="H300" s="33" t="s">
         <v>27</v>
@@ -14910,7 +14919,7 @@
         <v>2</v>
       </c>
       <c r="P300" s="38" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q300" s="38" t="n">
         <v>0</v>
@@ -14918,10 +14927,10 @@
     </row>
     <row r="301" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B301" s="21" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="C301" s="39" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="D301" s="1" t="n">
         <v>9</v>
@@ -14962,7 +14971,7 @@
         <v>2</v>
       </c>
       <c r="P301" s="38" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q301" s="38" t="n">
         <v>0</v>
@@ -14986,12 +14995,12 @@
       <c r="M302" s="25"/>
       <c r="N302" s="0"/>
     </row>
-    <row r="303" s="38" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B303" s="21" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="C303" s="39" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D303" s="1" t="n">
         <v>32</v>
@@ -15025,14 +15034,14 @@
         <f aca="false">J303/32</f>
         <v>9</v>
       </c>
-      <c r="N303" s="38" t="s">
-        <v>480</v>
+      <c r="N303" s="1" t="s">
+        <v>422</v>
       </c>
       <c r="O303" s="38" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P303" s="38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q303" s="38" t="n">
         <v>0</v>
@@ -15040,10 +15049,10 @@
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B304" s="21" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C304" s="21" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D304" s="1" t="n">
         <v>32</v>
@@ -15078,13 +15087,13 @@
         <v>10</v>
       </c>
       <c r="N304" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O304" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P304" s="38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q304" s="38" t="n">
         <v>0</v>
@@ -15092,10 +15101,10 @@
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B305" s="21" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C305" s="21" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D305" s="1" t="n">
         <v>32</v>
@@ -15130,13 +15139,13 @@
         <v>11</v>
       </c>
       <c r="N305" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O305" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P305" s="38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q305" s="38" t="n">
         <v>0</v>
@@ -15144,10 +15153,10 @@
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B306" s="21" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C306" s="21" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="D306" s="1" t="n">
         <v>32</v>
@@ -15182,13 +15191,13 @@
         <v>12</v>
       </c>
       <c r="N306" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O306" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P306" s="38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q306" s="38" t="n">
         <v>0</v>
@@ -15196,10 +15205,10 @@
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B307" s="21" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C307" s="21" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="D307" s="1" t="n">
         <v>32</v>
@@ -15234,13 +15243,13 @@
         <v>13</v>
       </c>
       <c r="N307" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O307" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P307" s="38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q307" s="38" t="n">
         <v>0</v>
@@ -15248,10 +15257,10 @@
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B308" s="21" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C308" s="21" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="D308" s="1" t="n">
         <v>8</v>
@@ -15286,13 +15295,13 @@
         <v>14</v>
       </c>
       <c r="N308" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O308" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P308" s="38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q308" s="38" t="n">
         <v>0</v>
@@ -15300,10 +15309,10 @@
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B309" s="21" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C309" s="21" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="D309" s="1" t="n">
         <v>8</v>
@@ -15338,13 +15347,13 @@
         <v>14.25</v>
       </c>
       <c r="N309" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O309" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P309" s="38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q309" s="38" t="n">
         <v>0</v>
@@ -15352,10 +15361,10 @@
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B310" s="21" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C310" s="21" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="D310" s="1" t="n">
         <v>8</v>
@@ -15390,13 +15399,13 @@
         <v>14.5</v>
       </c>
       <c r="N310" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O310" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P310" s="38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q310" s="38" t="n">
         <v>0</v>
@@ -15404,10 +15413,10 @@
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B311" s="21" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C311" s="21" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="D311" s="1" t="n">
         <v>8</v>
@@ -15442,13 +15451,13 @@
         <v>14.75</v>
       </c>
       <c r="N311" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O311" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P311" s="38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q311" s="38" t="n">
         <v>0</v>
@@ -15456,10 +15465,10 @@
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B312" s="21" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C312" s="21" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D312" s="1" t="n">
         <v>8</v>
@@ -15494,13 +15503,13 @@
         <v>15</v>
       </c>
       <c r="N312" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O312" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P312" s="38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q312" s="38" t="n">
         <v>0</v>
@@ -15508,10 +15517,10 @@
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B313" s="21" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C313" s="21" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D313" s="1" t="n">
         <v>8</v>
@@ -15546,13 +15555,13 @@
         <v>15.25</v>
       </c>
       <c r="N313" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O313" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P313" s="38" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q313" s="38" t="n">
         <v>0</v>
@@ -15560,10 +15569,10 @@
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B314" s="21" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C314" s="21" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D314" s="1" t="n">
         <v>8</v>
@@ -15598,13 +15607,13 @@
         <v>15.5</v>
       </c>
       <c r="N314" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O314" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P314" s="38" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q314" s="38" t="n">
         <v>0</v>
@@ -15612,10 +15621,10 @@
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B315" s="21" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C315" s="21" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D315" s="1" t="n">
         <v>8</v>
@@ -15650,13 +15659,13 @@
         <v>15.75</v>
       </c>
       <c r="N315" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O315" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P315" s="38" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q315" s="38" t="n">
         <v>0</v>
@@ -15664,10 +15673,10 @@
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B316" s="21" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C316" s="21" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D316" s="1" t="n">
         <v>8</v>
@@ -15702,13 +15711,13 @@
         <v>16</v>
       </c>
       <c r="N316" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O316" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P316" s="38" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q316" s="38" t="n">
         <v>0</v>
@@ -15716,10 +15725,10 @@
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B317" s="21" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="C317" s="21" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="D317" s="1" t="n">
         <v>8</v>
@@ -15754,13 +15763,13 @@
         <v>16.25</v>
       </c>
       <c r="N317" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O317" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P317" s="38" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q317" s="38" t="n">
         <v>0</v>
@@ -15768,10 +15777,10 @@
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B318" s="21" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C318" s="21" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D318" s="1" t="n">
         <v>8</v>
@@ -15806,13 +15815,13 @@
         <v>16.5</v>
       </c>
       <c r="N318" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O318" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P318" s="38" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q318" s="38" t="n">
         <v>0</v>
@@ -15820,10 +15829,10 @@
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B319" s="21" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="C319" s="21" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="D319" s="1" t="n">
         <v>8</v>
@@ -15858,13 +15867,13 @@
         <v>16.75</v>
       </c>
       <c r="N319" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O319" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P319" s="38" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q319" s="38" t="n">
         <v>0</v>
@@ -15872,10 +15881,10 @@
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B320" s="21" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="C320" s="21" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="D320" s="1" t="n">
         <v>8</v>
@@ -15910,13 +15919,13 @@
         <v>17</v>
       </c>
       <c r="N320" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O320" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P320" s="38" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q320" s="38" t="n">
         <v>0</v>
@@ -15924,10 +15933,10 @@
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B321" s="21" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C321" s="21" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="D321" s="1" t="n">
         <v>8</v>
@@ -15962,13 +15971,13 @@
         <v>17.25</v>
       </c>
       <c r="N321" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O321" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P321" s="38" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q321" s="38" t="n">
         <v>0</v>
@@ -15976,10 +15985,10 @@
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B322" s="21" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C322" s="21" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="D322" s="1" t="n">
         <v>8</v>
@@ -16014,13 +16023,13 @@
         <v>17.5</v>
       </c>
       <c r="N322" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O322" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P322" s="38" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q322" s="38" t="n">
         <v>0</v>
@@ -16028,10 +16037,10 @@
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B323" s="21" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C323" s="21" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="D323" s="1" t="n">
         <v>8</v>
@@ -16066,13 +16075,13 @@
         <v>17.75</v>
       </c>
       <c r="N323" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O323" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P323" s="38" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q323" s="38" t="n">
         <v>0</v>
@@ -16080,10 +16089,10 @@
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B324" s="21" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="C324" s="21" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="D324" s="1" t="n">
         <v>8</v>
@@ -16118,13 +16127,13 @@
         <v>18</v>
       </c>
       <c r="N324" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O324" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P324" s="38" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q324" s="38" t="n">
         <v>0</v>
@@ -16132,10 +16141,10 @@
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B325" s="21" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="C325" s="21" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="D325" s="1" t="n">
         <v>8</v>
@@ -16170,13 +16179,13 @@
         <v>18.25</v>
       </c>
       <c r="N325" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O325" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P325" s="38" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q325" s="38" t="n">
         <v>0</v>
@@ -16184,10 +16193,10 @@
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B326" s="21" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="C326" s="21" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="D326" s="1" t="n">
         <v>8</v>
@@ -16222,13 +16231,13 @@
         <v>18.5</v>
       </c>
       <c r="N326" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O326" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P326" s="38" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q326" s="38" t="n">
         <v>0</v>
@@ -16236,10 +16245,10 @@
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B327" s="21" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="C327" s="21" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="D327" s="1" t="n">
         <v>8</v>
@@ -16274,13 +16283,13 @@
         <v>18.75</v>
       </c>
       <c r="N327" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O327" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P327" s="38" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q327" s="38" t="n">
         <v>0</v>
@@ -16288,10 +16297,10 @@
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B328" s="21" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C328" s="21" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D328" s="1" t="n">
         <v>8</v>
@@ -16326,13 +16335,13 @@
         <v>19</v>
       </c>
       <c r="N328" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O328" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P328" s="38" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q328" s="38" t="n">
         <v>0</v>
@@ -16340,10 +16349,10 @@
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B329" s="21" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C329" s="21" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="D329" s="1" t="n">
         <v>8</v>
@@ -16378,13 +16387,13 @@
         <v>19.25</v>
       </c>
       <c r="N329" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O329" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P329" s="38" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q329" s="38" t="n">
         <v>0</v>
@@ -16392,10 +16401,10 @@
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B330" s="21" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="C330" s="21" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="D330" s="1" t="n">
         <v>8</v>
@@ -16430,13 +16439,13 @@
         <v>19.5</v>
       </c>
       <c r="N330" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O330" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P330" s="38" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q330" s="38" t="n">
         <v>0</v>
@@ -16444,10 +16453,10 @@
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B331" s="21" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C331" s="21" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="D331" s="1" t="n">
         <v>8</v>
@@ -16482,13 +16491,13 @@
         <v>19.75</v>
       </c>
       <c r="N331" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O331" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P331" s="38" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q331" s="38" t="n">
         <v>0</v>
@@ -16496,10 +16505,10 @@
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B332" s="21" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="C332" s="21" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="D332" s="1" t="n">
         <v>8</v>
@@ -16534,13 +16543,13 @@
         <v>20</v>
       </c>
       <c r="N332" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O332" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P332" s="38" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q332" s="38" t="n">
         <v>0</v>
@@ -16548,10 +16557,10 @@
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B333" s="21" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="C333" s="21" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="D333" s="1" t="n">
         <v>8</v>
@@ -16586,13 +16595,13 @@
         <v>20.25</v>
       </c>
       <c r="N333" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O333" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P333" s="38" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q333" s="38" t="n">
         <v>0</v>
@@ -16600,10 +16609,10 @@
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B334" s="21" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C334" s="21" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D334" s="1" t="n">
         <v>8</v>
@@ -16638,13 +16647,13 @@
         <v>20.5</v>
       </c>
       <c r="N334" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O334" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P334" s="38" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q334" s="38" t="n">
         <v>0</v>
@@ -16652,10 +16661,10 @@
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B335" s="21" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="C335" s="21" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="D335" s="1" t="n">
         <v>8</v>
@@ -16690,13 +16699,13 @@
         <v>20.75</v>
       </c>
       <c r="N335" s="38" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="O335" s="38" t="n">
         <v>4</v>
       </c>
       <c r="P335" s="38" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q335" s="38" t="n">
         <v>0</v>
@@ -16704,10 +16713,10 @@
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B336" s="3" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="C336" s="3" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D336" s="1" t="n">
         <v>16</v>
@@ -16744,13 +16753,13 @@
         <v>21</v>
       </c>
       <c r="N336" s="38" t="s">
-        <v>480</v>
+        <v>402</v>
       </c>
       <c r="O336" s="38" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P336" s="38" t="n">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="Q336" s="38" t="n">
         <v>0</v>
@@ -16767,7 +16776,7 @@
         <v>16</v>
       </c>
       <c r="E337" s="33" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="F337" s="33"/>
       <c r="G337" s="33" t="n">
@@ -16835,7 +16844,7 @@
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="36" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="F339" s="33"/>
       <c r="G339" s="33"/>
@@ -16918,10 +16927,10 @@
     </row>
     <row r="342" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B342" s="21" t="s">
-        <v>420</v>
+        <v>550</v>
       </c>
       <c r="C342" s="39" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="D342" s="1" t="n">
         <v>9</v>
@@ -16973,7 +16982,7 @@
         <v>423</v>
       </c>
       <c r="C343" s="39" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="D343" s="1" t="n">
         <v>5</v>
@@ -16991,7 +17000,7 @@
       <c r="I343" s="33" t="s">
         <v>405</v>
       </c>
-      <c r="J343" s="37" t="n">
+      <c r="J343" s="4" t="n">
         <f aca="false">J342+D342</f>
         <v>713</v>
       </c>
@@ -17025,7 +17034,7 @@
         <v>425</v>
       </c>
       <c r="C344" s="39" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="D344" s="1" t="n">
         <v>4</v>
@@ -17043,7 +17052,7 @@
       <c r="I344" s="33" t="s">
         <v>405</v>
       </c>
-      <c r="J344" s="37" t="n">
+      <c r="J344" s="4" t="n">
         <f aca="false">J343+D343</f>
         <v>718</v>
       </c>
@@ -17077,7 +17086,7 @@
         <v>427</v>
       </c>
       <c r="C345" s="39" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="D345" s="1" t="n">
         <v>4</v>
@@ -17095,7 +17104,7 @@
       <c r="I345" s="33" t="s">
         <v>405</v>
       </c>
-      <c r="J345" s="37" t="n">
+      <c r="J345" s="4" t="n">
         <f aca="false">J344+D344</f>
         <v>722</v>
       </c>
@@ -17129,7 +17138,7 @@
         <v>429</v>
       </c>
       <c r="C346" s="39" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="D346" s="1" t="n">
         <v>3</v>
@@ -17147,7 +17156,7 @@
       <c r="I346" s="33" t="s">
         <v>405</v>
       </c>
-      <c r="J346" s="37" t="n">
+      <c r="J346" s="4" t="n">
         <f aca="false">J345+D345</f>
         <v>726</v>
       </c>
@@ -17181,7 +17190,7 @@
         <v>431</v>
       </c>
       <c r="C347" s="39" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="D347" s="1" t="n">
         <v>1</v>
@@ -17199,7 +17208,7 @@
       <c r="I347" s="33" t="s">
         <v>405</v>
       </c>
-      <c r="J347" s="37" t="n">
+      <c r="J347" s="4" t="n">
         <f aca="false">J346+D346</f>
         <v>729</v>
       </c>
@@ -17230,10 +17239,10 @@
     </row>
     <row r="348" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B348" s="21" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="C348" s="39" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="D348" s="1" t="n">
         <v>1</v>
@@ -17251,7 +17260,7 @@
       <c r="I348" s="33" t="s">
         <v>405</v>
       </c>
-      <c r="J348" s="37" t="n">
+      <c r="J348" s="4" t="n">
         <f aca="false">J347+D347</f>
         <v>730</v>
       </c>
@@ -17285,10 +17294,10 @@
         <v>436</v>
       </c>
       <c r="C349" s="39" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="D349" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E349" s="33" t="s">
         <v>26</v>
@@ -17303,21 +17312,21 @@
       <c r="I349" s="33" t="s">
         <v>405</v>
       </c>
-      <c r="J349" s="37" t="n">
-        <f aca="false">J347+D347</f>
-        <v>730</v>
+      <c r="J349" s="4" t="n">
+        <f aca="false">J348+D348</f>
+        <v>731</v>
       </c>
       <c r="K349" s="25" t="n">
         <f aca="false">J349/8</f>
-        <v>91.25</v>
+        <v>91.375</v>
       </c>
       <c r="L349" s="25" t="n">
         <f aca="false">J349/16</f>
-        <v>45.625</v>
+        <v>45.6875</v>
       </c>
       <c r="M349" s="25" t="n">
         <f aca="false">J349/32</f>
-        <v>22.8125</v>
+        <v>22.84375</v>
       </c>
       <c r="N349" s="38" t="s">
         <v>29</v>
@@ -17344,10 +17353,22 @@
       <c r="G350" s="33"/>
       <c r="H350" s="33"/>
       <c r="I350" s="33"/>
-      <c r="J350" s="37"/>
-      <c r="K350" s="25"/>
-      <c r="L350" s="25"/>
-      <c r="M350" s="25"/>
+      <c r="J350" s="4" t="n">
+        <f aca="false">J349+D349</f>
+        <v>736</v>
+      </c>
+      <c r="K350" s="25" t="n">
+        <f aca="false">J350/8</f>
+        <v>92</v>
+      </c>
+      <c r="L350" s="25" t="n">
+        <f aca="false">J350/16</f>
+        <v>46</v>
+      </c>
+      <c r="M350" s="25" t="n">
+        <f aca="false">J350/32</f>
+        <v>23</v>
+      </c>
     </row>
     <row r="351" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="38" t="s">
@@ -17371,7 +17392,7 @@
         <v>436</v>
       </c>
       <c r="C352" s="39" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="D352" s="1" t="n">
         <v>5</v>
@@ -17420,10 +17441,10 @@
     </row>
     <row r="353" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B353" s="21" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="C353" s="39" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="D353" s="1" t="n">
         <v>1</v>
@@ -17475,7 +17496,7 @@
         <v>431</v>
       </c>
       <c r="C354" s="39" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="D354" s="1" t="n">
         <v>1</v>
@@ -17516,7 +17537,7 @@
         <v>2</v>
       </c>
       <c r="P354" s="38" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="Q354" s="38" t="n">
         <v>0</v>
@@ -17527,7 +17548,7 @@
         <v>429</v>
       </c>
       <c r="C355" s="39" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="D355" s="1" t="n">
         <v>3</v>
@@ -17568,7 +17589,7 @@
         <v>2</v>
       </c>
       <c r="P355" s="38" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="Q355" s="38" t="n">
         <v>0</v>
@@ -17579,7 +17600,7 @@
         <v>427</v>
       </c>
       <c r="C356" s="39" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="D356" s="1" t="n">
         <v>4</v>
@@ -17620,7 +17641,7 @@
         <v>2</v>
       </c>
       <c r="P356" s="38" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="Q356" s="38" t="n">
         <v>0</v>
@@ -17631,7 +17652,7 @@
         <v>425</v>
       </c>
       <c r="C357" s="39" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="D357" s="1" t="n">
         <v>4</v>
@@ -17672,7 +17693,7 @@
         <v>2</v>
       </c>
       <c r="P357" s="38" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="Q357" s="38" t="n">
         <v>0</v>
@@ -17683,7 +17704,7 @@
         <v>423</v>
       </c>
       <c r="C358" s="39" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="D358" s="1" t="n">
         <v>5</v>
@@ -17693,7 +17714,7 @@
       </c>
       <c r="F358" s="40"/>
       <c r="G358" s="33" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="H358" s="33" t="s">
         <v>27</v>
@@ -17724,7 +17745,7 @@
         <v>2</v>
       </c>
       <c r="P358" s="38" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Q358" s="38" t="n">
         <v>0</v>
@@ -17732,10 +17753,10 @@
     </row>
     <row r="359" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B359" s="21" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="C359" s="39" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="D359" s="1" t="n">
         <v>9</v>
@@ -17776,7 +17797,7 @@
         <v>2</v>
       </c>
       <c r="P359" s="38" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Q359" s="38" t="n">
         <v>0</v>
@@ -17799,15 +17820,15 @@
       <c r="L360" s="25"/>
       <c r="M360" s="25"/>
       <c r="N360" s="38" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="361" s="38" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="361" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B361" s="21" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="C361" s="39" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="D361" s="1" t="n">
         <v>32</v>
@@ -17842,13 +17863,13 @@
         <v>23</v>
       </c>
       <c r="N361" s="38" t="s">
-        <v>558</v>
+        <v>422</v>
       </c>
       <c r="O361" s="38" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P361" s="38" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="Q361" s="38" t="n">
         <v>0</v>
@@ -17857,10 +17878,10 @@
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="38"/>
       <c r="B362" s="21" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C362" s="21" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="D362" s="1" t="n">
         <v>32</v>
@@ -17895,13 +17916,13 @@
         <v>24</v>
       </c>
       <c r="N362" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O362" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P362" s="38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q362" s="38" t="n">
         <v>0</v>
@@ -17909,10 +17930,10 @@
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B363" s="21" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C363" s="21" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="D363" s="1" t="n">
         <v>32</v>
@@ -17947,13 +17968,13 @@
         <v>25</v>
       </c>
       <c r="N363" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O363" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P363" s="38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q363" s="38" t="n">
         <v>0</v>
@@ -17961,10 +17982,10 @@
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B364" s="21" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="C364" s="21" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="D364" s="1" t="n">
         <v>32</v>
@@ -17999,13 +18020,13 @@
         <v>26</v>
       </c>
       <c r="N364" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O364" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P364" s="38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q364" s="38" t="n">
         <v>0</v>
@@ -18013,10 +18034,10 @@
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B365" s="21" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="C365" s="21" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D365" s="1" t="n">
         <v>32</v>
@@ -18051,13 +18072,13 @@
         <v>27</v>
       </c>
       <c r="N365" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O365" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P365" s="38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q365" s="38" t="n">
         <v>0</v>
@@ -18065,10 +18086,10 @@
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B366" s="21" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="C366" s="21" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D366" s="1" t="n">
         <v>8</v>
@@ -18103,13 +18124,13 @@
         <v>28</v>
       </c>
       <c r="N366" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O366" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P366" s="38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q366" s="38" t="n">
         <v>0</v>
@@ -18117,10 +18138,10 @@
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B367" s="21" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="C367" s="21" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="D367" s="1" t="n">
         <v>8</v>
@@ -18155,13 +18176,13 @@
         <v>28.25</v>
       </c>
       <c r="N367" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O367" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P367" s="38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q367" s="38" t="n">
         <v>0</v>
@@ -18169,10 +18190,10 @@
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B368" s="21" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C368" s="21" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="D368" s="1" t="n">
         <v>8</v>
@@ -18207,13 +18228,13 @@
         <v>28.5</v>
       </c>
       <c r="N368" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O368" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P368" s="38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q368" s="38" t="n">
         <v>0</v>
@@ -18221,10 +18242,10 @@
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B369" s="21" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C369" s="21" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="D369" s="1" t="n">
         <v>8</v>
@@ -18259,13 +18280,13 @@
         <v>28.75</v>
       </c>
       <c r="N369" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O369" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P369" s="38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q369" s="38" t="n">
         <v>0</v>
@@ -18273,10 +18294,10 @@
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B370" s="21" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="C370" s="21" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="D370" s="1" t="n">
         <v>8</v>
@@ -18311,13 +18332,13 @@
         <v>29</v>
       </c>
       <c r="N370" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O370" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P370" s="38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q370" s="38" t="n">
         <v>0</v>
@@ -18325,10 +18346,10 @@
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B371" s="21" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C371" s="21" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="D371" s="1" t="n">
         <v>8</v>
@@ -18363,13 +18384,13 @@
         <v>29.25</v>
       </c>
       <c r="N371" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O371" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P371" s="38" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q371" s="38" t="n">
         <v>0</v>
@@ -18377,10 +18398,10 @@
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B372" s="21" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C372" s="21" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="D372" s="1" t="n">
         <v>8</v>
@@ -18415,13 +18436,13 @@
         <v>29.5</v>
       </c>
       <c r="N372" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O372" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P372" s="38" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q372" s="38" t="n">
         <v>0</v>
@@ -18429,10 +18450,10 @@
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B373" s="21" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C373" s="21" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="D373" s="1" t="n">
         <v>8</v>
@@ -18467,13 +18488,13 @@
         <v>29.75</v>
       </c>
       <c r="N373" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O373" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P373" s="38" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q373" s="38" t="n">
         <v>0</v>
@@ -18481,10 +18502,10 @@
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B374" s="21" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="C374" s="21" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="D374" s="1" t="n">
         <v>8</v>
@@ -18519,13 +18540,13 @@
         <v>30</v>
       </c>
       <c r="N374" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O374" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P374" s="38" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q374" s="38" t="n">
         <v>0</v>
@@ -18533,10 +18554,10 @@
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B375" s="21" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C375" s="21" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="D375" s="1" t="n">
         <v>8</v>
@@ -18571,13 +18592,13 @@
         <v>30.25</v>
       </c>
       <c r="N375" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O375" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P375" s="38" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q375" s="38" t="n">
         <v>0</v>
@@ -18585,10 +18606,10 @@
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B376" s="21" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="C376" s="21" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="D376" s="1" t="n">
         <v>8</v>
@@ -18623,13 +18644,13 @@
         <v>30.5</v>
       </c>
       <c r="N376" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O376" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P376" s="38" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q376" s="38" t="n">
         <v>0</v>
@@ -18637,10 +18658,10 @@
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B377" s="21" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C377" s="21" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="D377" s="1" t="n">
         <v>8</v>
@@ -18675,13 +18696,13 @@
         <v>30.75</v>
       </c>
       <c r="N377" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O377" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P377" s="38" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q377" s="38" t="n">
         <v>0</v>
@@ -18689,10 +18710,10 @@
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B378" s="21" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C378" s="21" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="D378" s="1" t="n">
         <v>8</v>
@@ -18727,13 +18748,13 @@
         <v>31</v>
       </c>
       <c r="N378" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O378" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P378" s="38" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q378" s="38" t="n">
         <v>0</v>
@@ -18741,10 +18762,10 @@
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B379" s="21" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="C379" s="21" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="D379" s="1" t="n">
         <v>8</v>
@@ -18779,13 +18800,13 @@
         <v>31.25</v>
       </c>
       <c r="N379" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O379" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P379" s="38" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q379" s="38" t="n">
         <v>0</v>
@@ -18793,10 +18814,10 @@
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B380" s="21" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="C380" s="21" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D380" s="1" t="n">
         <v>8</v>
@@ -18831,13 +18852,13 @@
         <v>31.5</v>
       </c>
       <c r="N380" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O380" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P380" s="38" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q380" s="38" t="n">
         <v>0</v>
@@ -18845,10 +18866,10 @@
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B381" s="21" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C381" s="21" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="D381" s="1" t="n">
         <v>8</v>
@@ -18883,13 +18904,13 @@
         <v>31.75</v>
       </c>
       <c r="N381" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O381" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P381" s="38" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q381" s="38" t="n">
         <v>0</v>
@@ -18897,10 +18918,10 @@
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B382" s="21" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="C382" s="21" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="D382" s="1" t="n">
         <v>8</v>
@@ -18935,13 +18956,13 @@
         <v>32</v>
       </c>
       <c r="N382" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O382" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P382" s="38" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q382" s="38" t="n">
         <v>0</v>
@@ -18949,10 +18970,10 @@
     </row>
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B383" s="21" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="C383" s="21" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="D383" s="1" t="n">
         <v>8</v>
@@ -18987,13 +19008,13 @@
         <v>32.25</v>
       </c>
       <c r="N383" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O383" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P383" s="38" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q383" s="38" t="n">
         <v>0</v>
@@ -19001,10 +19022,10 @@
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B384" s="21" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C384" s="21" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="D384" s="1" t="n">
         <v>8</v>
@@ -19039,13 +19060,13 @@
         <v>32.5</v>
       </c>
       <c r="N384" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O384" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P384" s="38" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q384" s="38" t="n">
         <v>0</v>
@@ -19053,10 +19074,10 @@
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B385" s="21" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="C385" s="21" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="D385" s="1" t="n">
         <v>8</v>
@@ -19091,13 +19112,13 @@
         <v>32.75</v>
       </c>
       <c r="N385" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O385" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P385" s="38" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q385" s="38" t="n">
         <v>0</v>
@@ -19105,10 +19126,10 @@
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B386" s="21" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="C386" s="21" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="D386" s="1" t="n">
         <v>8</v>
@@ -19143,13 +19164,13 @@
         <v>33</v>
       </c>
       <c r="N386" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O386" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P386" s="38" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q386" s="38" t="n">
         <v>0</v>
@@ -19157,10 +19178,10 @@
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B387" s="21" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C387" s="21" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="D387" s="1" t="n">
         <v>8</v>
@@ -19195,13 +19216,13 @@
         <v>33.25</v>
       </c>
       <c r="N387" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O387" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P387" s="38" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q387" s="38" t="n">
         <v>0</v>
@@ -19209,10 +19230,10 @@
     </row>
     <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B388" s="21" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="C388" s="21" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D388" s="1" t="n">
         <v>8</v>
@@ -19247,13 +19268,13 @@
         <v>33.5</v>
       </c>
       <c r="N388" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O388" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P388" s="38" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q388" s="38" t="n">
         <v>0</v>
@@ -19261,10 +19282,10 @@
     </row>
     <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B389" s="21" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="C389" s="21" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="D389" s="1" t="n">
         <v>8</v>
@@ -19299,13 +19320,13 @@
         <v>33.75</v>
       </c>
       <c r="N389" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O389" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P389" s="38" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q389" s="38" t="n">
         <v>0</v>
@@ -19313,10 +19334,10 @@
     </row>
     <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B390" s="21" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="C390" s="21" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="D390" s="1" t="n">
         <v>8</v>
@@ -19351,13 +19372,13 @@
         <v>34</v>
       </c>
       <c r="N390" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O390" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P390" s="38" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q390" s="38" t="n">
         <v>0</v>
@@ -19365,10 +19386,10 @@
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B391" s="21" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="C391" s="21" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="D391" s="1" t="n">
         <v>8</v>
@@ -19403,13 +19424,13 @@
         <v>34.25</v>
       </c>
       <c r="N391" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O391" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P391" s="38" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q391" s="38" t="n">
         <v>0</v>
@@ -19417,10 +19438,10 @@
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B392" s="21" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="C392" s="21" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="D392" s="1" t="n">
         <v>8</v>
@@ -19455,13 +19476,13 @@
         <v>34.5</v>
       </c>
       <c r="N392" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O392" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P392" s="38" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q392" s="38" t="n">
         <v>0</v>
@@ -19469,10 +19490,10 @@
     </row>
     <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B393" s="21" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="C393" s="21" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="D393" s="1" t="n">
         <v>8</v>
@@ -19507,13 +19528,13 @@
         <v>34.75</v>
       </c>
       <c r="N393" s="38" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="O393" s="38" t="n">
         <v>5</v>
       </c>
       <c r="P393" s="38" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q393" s="38" t="n">
         <v>0</v>
@@ -19521,10 +19542,10 @@
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B394" s="3" t="s">
-        <v>545</v>
+        <v>625</v>
       </c>
       <c r="C394" s="3" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D394" s="1" t="n">
         <v>16</v>
@@ -19561,13 +19582,13 @@
         <v>35</v>
       </c>
       <c r="N394" s="38" t="s">
-        <v>558</v>
+        <v>402</v>
       </c>
       <c r="O394" s="38" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P394" s="38" t="n">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="Q394" s="38" t="n">
         <v>0</v>
@@ -19584,7 +19605,7 @@
         <v>16</v>
       </c>
       <c r="E395" s="33" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="F395" s="33"/>
       <c r="G395" s="33" t="n">
@@ -19689,10 +19710,10 @@
   <dimension ref="B6:I20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="1" sqref="N295 F8"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.11"/>
@@ -19702,22 +19723,22 @@
     <row r="6" s="43" customFormat="true" ht="34.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="44"/>
       <c r="C6" s="44" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="F6" s="44" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="G6" s="44" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="I6" s="44"/>
     </row>

</xml_diff>

<commit_message>
Minor update to fix version numbers
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecGolf-T.xlsx
+++ b/genSpacecraft/DownlinkSpecGolf-T.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2190" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2190" uniqueCount="634">
   <si>
     <t xml:space="preserve">//</t>
   </si>
@@ -1418,255 +1418,258 @@
     <t xml:space="preserve">LIHU Version Number</t>
   </si>
   <si>
+    <t xml:space="preserve">LegSWVersion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LegErrorData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure:rt1Errors_t,file:rt1ErrorsDownlink.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watchdog Tasks Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wdReports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errorCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taskNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">previousTask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">earlyResetCount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wasStillEarlyInBoot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTIHU1 Data Valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filler1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOLF_RTIHU_ERR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTIHU1: WD Tasks Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errorData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary SRAM Corrected Addr 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAMCorAddr1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary RT Errors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary SRAM Corrected Addr 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAMCorAddr2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Flash Corrected Addr 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROMCorAddr1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Flash Corrected Addr 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROMCorAddr2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCT1CmdFailCRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCTCmdFailCRCCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCT1CmdFailTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCTCmdFailTimeCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCT1CmdFailAuthenticate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCTCmdFailAuthenticateCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCT1CmdFailCommand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCTCmdFailCommandCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCT1CmdFailNamespace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCTCmdFailNamespaceCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1I2C1Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C1ErrorCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1I2C2Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C2ErrorCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1I2C1Reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C1ResetCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1I2C2Reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C2ResetCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1 I2c1 Retry Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C1RetryCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1 I2c2 Retry Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C2RetryCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1SPIRetries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPIRetryCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1 MRAM CRC Fail count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MramCRCCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1 MRAM Read Error Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MramRdErrorCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1 MRAM Write Error Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MramWtErrorCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1FlashCorrectable Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FlashCorCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1 Ram Even Bank Correctable Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RamEvenCorCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1 Ram Odd Bank Correctable Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RamOddCorCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1PLLSlip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLLSlipCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1ClockMonitorFail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClockMonitorFailCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1VIMRamParity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIMRamParityCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1CAN1RamParity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN1RamParityCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1CAN2RamParity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN2RamParityCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1DCC1Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCC1ErrorCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1DCC2Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCC2ErrorCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1N2HET2RamParity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N2HET2RamParityCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT1IOMMAccvio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOMMAccvioCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-fatal error count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nonFatalCnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTIHU1 Version Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">SWVersion</t>
   </si>
   <si>
-    <t xml:space="preserve">Error Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LegErrorData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure:rt1Errors_t,file:rt1ErrorsDownlink.h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watchdog Tasks Ok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wdReports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">errorCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">taskNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">previousTask</t>
-  </si>
-  <si>
-    <t xml:space="preserve">earlyResetCount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wasStillEarlyInBoot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTIHU1 Data Valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">filler1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOLF_RTIHU_ERR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTIHU1: WD Tasks Ok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">errorData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary SRAM Corrected Addr 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAMCorAddr1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary RT Errors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary SRAM Corrected Addr 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAMCorAddr2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary Flash Corrected Addr 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROMCorAddr1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary Flash Corrected Addr 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROMCorAddr2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCT1CmdFailCRC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCTCmdFailCRCCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCT1CmdFailTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCTCmdFailTimeCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCT1CmdFailAuthenticate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCTCmdFailAuthenticateCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCT1CmdFailCommand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCTCmdFailCommandCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCT1CmdFailNamespace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCTCmdFailNamespaceCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1I2C1Error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C1ErrorCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1I2C2Error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C2ErrorCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1I2C1Reset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C1ResetCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1I2C2Reset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C2ResetCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1 I2c1 Retry Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C1RetryCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1 I2c2 Retry Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C2RetryCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1SPIRetries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPIRetryCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1 MRAM CRC Fail count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MramCRCCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1 MRAM Read Error Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MramRdErrorCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1 MRAM Write Error Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MramWtErrorCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1FlashCorrectable Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FlashCorCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1 Ram Even Bank Correctable Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RamEvenCorCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1 Ram Odd Bank Correctable Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RamOddCorCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1PLLSlip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLLSlipCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1ClockMonitorFail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClockMonitorFailCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1VIMRamParity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VIMRamParityCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1CAN1RamParity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAN1RamParityCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1CAN2RamParity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAN2RamParityCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1DCC1Error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCC1ErrorCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1DCC2Error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCC2ErrorCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1N2HET2RamParity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2HET2RamParityCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1IOMMAccvio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOMMAccvioCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-fatal error count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nonFatalCnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTIHU1 Version Number</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unisgned</t>
   </si>
   <si>
@@ -1899,6 +1902,9 @@
   </si>
   <si>
     <t xml:space="preserve">RTIHU2 Version Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT2SWVersion</t>
   </si>
   <si>
     <t xml:space="preserve">Payloads per Frame</t>
@@ -2266,8 +2272,8 @@
   </sheetPr>
   <dimension ref="A1:Q397"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A275" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J361" activeCellId="0" sqref="J361"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A278" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C394" activeCellId="0" sqref="C394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16716,7 +16722,7 @@
         <v>547</v>
       </c>
       <c r="C336" s="3" t="s">
-        <v>465</v>
+        <v>548</v>
       </c>
       <c r="D336" s="1" t="n">
         <v>16</v>
@@ -16776,7 +16782,7 @@
         <v>16</v>
       </c>
       <c r="E337" s="33" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F337" s="33"/>
       <c r="G337" s="33" t="n">
@@ -16844,7 +16850,7 @@
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="36" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="F339" s="33"/>
       <c r="G339" s="33"/>
@@ -16927,10 +16933,10 @@
     </row>
     <row r="342" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B342" s="21" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C342" s="39" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D342" s="1" t="n">
         <v>9</v>
@@ -16982,7 +16988,7 @@
         <v>423</v>
       </c>
       <c r="C343" s="39" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="D343" s="1" t="n">
         <v>5</v>
@@ -17034,7 +17040,7 @@
         <v>425</v>
       </c>
       <c r="C344" s="39" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D344" s="1" t="n">
         <v>4</v>
@@ -17086,7 +17092,7 @@
         <v>427</v>
       </c>
       <c r="C345" s="39" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D345" s="1" t="n">
         <v>4</v>
@@ -17138,7 +17144,7 @@
         <v>429</v>
       </c>
       <c r="C346" s="39" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D346" s="1" t="n">
         <v>3</v>
@@ -17190,7 +17196,7 @@
         <v>431</v>
       </c>
       <c r="C347" s="39" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D347" s="1" t="n">
         <v>1</v>
@@ -17239,10 +17245,10 @@
     </row>
     <row r="348" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B348" s="21" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C348" s="39" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D348" s="1" t="n">
         <v>1</v>
@@ -17294,7 +17300,7 @@
         <v>436</v>
       </c>
       <c r="C349" s="39" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D349" s="1" t="n">
         <v>5</v>
@@ -17392,7 +17398,7 @@
         <v>436</v>
       </c>
       <c r="C352" s="39" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D352" s="1" t="n">
         <v>5</v>
@@ -17441,10 +17447,10 @@
     </row>
     <row r="353" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B353" s="21" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C353" s="39" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D353" s="1" t="n">
         <v>1</v>
@@ -17496,7 +17502,7 @@
         <v>431</v>
       </c>
       <c r="C354" s="39" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D354" s="1" t="n">
         <v>1</v>
@@ -17548,7 +17554,7 @@
         <v>429</v>
       </c>
       <c r="C355" s="39" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D355" s="1" t="n">
         <v>3</v>
@@ -17600,7 +17606,7 @@
         <v>427</v>
       </c>
       <c r="C356" s="39" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D356" s="1" t="n">
         <v>4</v>
@@ -17652,7 +17658,7 @@
         <v>425</v>
       </c>
       <c r="C357" s="39" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D357" s="1" t="n">
         <v>4</v>
@@ -17704,7 +17710,7 @@
         <v>423</v>
       </c>
       <c r="C358" s="39" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="D358" s="1" t="n">
         <v>5</v>
@@ -17753,10 +17759,10 @@
     </row>
     <row r="359" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B359" s="21" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C359" s="39" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D359" s="1" t="n">
         <v>9</v>
@@ -17820,7 +17826,7 @@
       <c r="L360" s="25"/>
       <c r="M360" s="25"/>
       <c r="N360" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="361" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17828,7 +17834,7 @@
         <v>466</v>
       </c>
       <c r="C361" s="39" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="D361" s="1" t="n">
         <v>32</v>
@@ -17878,10 +17884,10 @@
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="38"/>
       <c r="B362" s="21" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C362" s="21" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D362" s="1" t="n">
         <v>32</v>
@@ -17916,7 +17922,7 @@
         <v>24</v>
       </c>
       <c r="N362" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O362" s="38" t="n">
         <v>5</v>
@@ -17930,10 +17936,10 @@
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B363" s="21" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C363" s="21" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D363" s="1" t="n">
         <v>32</v>
@@ -17968,7 +17974,7 @@
         <v>25</v>
       </c>
       <c r="N363" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O363" s="38" t="n">
         <v>5</v>
@@ -17982,10 +17988,10 @@
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B364" s="21" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C364" s="21" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D364" s="1" t="n">
         <v>32</v>
@@ -18020,7 +18026,7 @@
         <v>26</v>
       </c>
       <c r="N364" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O364" s="38" t="n">
         <v>5</v>
@@ -18034,10 +18040,10 @@
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B365" s="21" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C365" s="21" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D365" s="1" t="n">
         <v>32</v>
@@ -18072,7 +18078,7 @@
         <v>27</v>
       </c>
       <c r="N365" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O365" s="38" t="n">
         <v>5</v>
@@ -18086,10 +18092,10 @@
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B366" s="21" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C366" s="21" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="D366" s="1" t="n">
         <v>8</v>
@@ -18124,7 +18130,7 @@
         <v>28</v>
       </c>
       <c r="N366" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O366" s="38" t="n">
         <v>5</v>
@@ -18138,10 +18144,10 @@
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B367" s="21" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C367" s="21" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="D367" s="1" t="n">
         <v>8</v>
@@ -18176,7 +18182,7 @@
         <v>28.25</v>
       </c>
       <c r="N367" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O367" s="38" t="n">
         <v>5</v>
@@ -18190,10 +18196,10 @@
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B368" s="21" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C368" s="21" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D368" s="1" t="n">
         <v>8</v>
@@ -18228,7 +18234,7 @@
         <v>28.5</v>
       </c>
       <c r="N368" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O368" s="38" t="n">
         <v>5</v>
@@ -18242,10 +18248,10 @@
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B369" s="21" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C369" s="21" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="D369" s="1" t="n">
         <v>8</v>
@@ -18280,7 +18286,7 @@
         <v>28.75</v>
       </c>
       <c r="N369" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O369" s="38" t="n">
         <v>5</v>
@@ -18294,10 +18300,10 @@
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B370" s="21" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C370" s="21" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D370" s="1" t="n">
         <v>8</v>
@@ -18332,7 +18338,7 @@
         <v>29</v>
       </c>
       <c r="N370" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O370" s="38" t="n">
         <v>5</v>
@@ -18346,10 +18352,10 @@
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B371" s="21" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C371" s="21" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D371" s="1" t="n">
         <v>8</v>
@@ -18384,7 +18390,7 @@
         <v>29.25</v>
       </c>
       <c r="N371" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O371" s="38" t="n">
         <v>5</v>
@@ -18398,10 +18404,10 @@
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B372" s="21" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C372" s="21" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D372" s="1" t="n">
         <v>8</v>
@@ -18436,7 +18442,7 @@
         <v>29.5</v>
       </c>
       <c r="N372" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O372" s="38" t="n">
         <v>5</v>
@@ -18450,10 +18456,10 @@
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B373" s="21" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C373" s="21" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D373" s="1" t="n">
         <v>8</v>
@@ -18488,7 +18494,7 @@
         <v>29.75</v>
       </c>
       <c r="N373" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O373" s="38" t="n">
         <v>5</v>
@@ -18502,10 +18508,10 @@
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B374" s="21" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C374" s="21" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D374" s="1" t="n">
         <v>8</v>
@@ -18540,7 +18546,7 @@
         <v>30</v>
       </c>
       <c r="N374" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O374" s="38" t="n">
         <v>5</v>
@@ -18554,10 +18560,10 @@
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B375" s="21" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C375" s="21" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D375" s="1" t="n">
         <v>8</v>
@@ -18592,7 +18598,7 @@
         <v>30.25</v>
       </c>
       <c r="N375" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O375" s="38" t="n">
         <v>5</v>
@@ -18606,10 +18612,10 @@
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B376" s="21" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C376" s="21" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D376" s="1" t="n">
         <v>8</v>
@@ -18644,7 +18650,7 @@
         <v>30.5</v>
       </c>
       <c r="N376" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O376" s="38" t="n">
         <v>5</v>
@@ -18658,10 +18664,10 @@
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B377" s="21" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C377" s="21" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D377" s="1" t="n">
         <v>8</v>
@@ -18696,7 +18702,7 @@
         <v>30.75</v>
       </c>
       <c r="N377" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O377" s="38" t="n">
         <v>5</v>
@@ -18710,10 +18716,10 @@
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B378" s="21" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C378" s="21" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D378" s="1" t="n">
         <v>8</v>
@@ -18748,7 +18754,7 @@
         <v>31</v>
       </c>
       <c r="N378" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O378" s="38" t="n">
         <v>5</v>
@@ -18762,10 +18768,10 @@
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B379" s="21" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C379" s="21" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D379" s="1" t="n">
         <v>8</v>
@@ -18800,7 +18806,7 @@
         <v>31.25</v>
       </c>
       <c r="N379" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O379" s="38" t="n">
         <v>5</v>
@@ -18814,10 +18820,10 @@
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B380" s="21" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C380" s="21" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D380" s="1" t="n">
         <v>8</v>
@@ -18852,7 +18858,7 @@
         <v>31.5</v>
       </c>
       <c r="N380" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O380" s="38" t="n">
         <v>5</v>
@@ -18866,10 +18872,10 @@
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B381" s="21" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C381" s="21" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D381" s="1" t="n">
         <v>8</v>
@@ -18904,7 +18910,7 @@
         <v>31.75</v>
       </c>
       <c r="N381" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O381" s="38" t="n">
         <v>5</v>
@@ -18918,10 +18924,10 @@
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B382" s="21" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="C382" s="21" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D382" s="1" t="n">
         <v>8</v>
@@ -18956,7 +18962,7 @@
         <v>32</v>
       </c>
       <c r="N382" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O382" s="38" t="n">
         <v>5</v>
@@ -18970,10 +18976,10 @@
     </row>
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B383" s="21" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="C383" s="21" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D383" s="1" t="n">
         <v>8</v>
@@ -19008,7 +19014,7 @@
         <v>32.25</v>
       </c>
       <c r="N383" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O383" s="38" t="n">
         <v>5</v>
@@ -19022,10 +19028,10 @@
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B384" s="21" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C384" s="21" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D384" s="1" t="n">
         <v>8</v>
@@ -19060,7 +19066,7 @@
         <v>32.5</v>
       </c>
       <c r="N384" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O384" s="38" t="n">
         <v>5</v>
@@ -19074,10 +19080,10 @@
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B385" s="21" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C385" s="21" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D385" s="1" t="n">
         <v>8</v>
@@ -19112,7 +19118,7 @@
         <v>32.75</v>
       </c>
       <c r="N385" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O385" s="38" t="n">
         <v>5</v>
@@ -19126,10 +19132,10 @@
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B386" s="21" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C386" s="21" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D386" s="1" t="n">
         <v>8</v>
@@ -19164,7 +19170,7 @@
         <v>33</v>
       </c>
       <c r="N386" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O386" s="38" t="n">
         <v>5</v>
@@ -19178,10 +19184,10 @@
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B387" s="21" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C387" s="21" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D387" s="1" t="n">
         <v>8</v>
@@ -19216,7 +19222,7 @@
         <v>33.25</v>
       </c>
       <c r="N387" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O387" s="38" t="n">
         <v>5</v>
@@ -19230,10 +19236,10 @@
     </row>
     <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B388" s="21" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C388" s="21" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D388" s="1" t="n">
         <v>8</v>
@@ -19268,7 +19274,7 @@
         <v>33.5</v>
       </c>
       <c r="N388" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O388" s="38" t="n">
         <v>5</v>
@@ -19282,10 +19288,10 @@
     </row>
     <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B389" s="21" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C389" s="21" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D389" s="1" t="n">
         <v>8</v>
@@ -19320,7 +19326,7 @@
         <v>33.75</v>
       </c>
       <c r="N389" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O389" s="38" t="n">
         <v>5</v>
@@ -19334,10 +19340,10 @@
     </row>
     <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B390" s="21" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C390" s="21" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D390" s="1" t="n">
         <v>8</v>
@@ -19372,7 +19378,7 @@
         <v>34</v>
       </c>
       <c r="N390" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O390" s="38" t="n">
         <v>5</v>
@@ -19386,10 +19392,10 @@
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B391" s="21" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C391" s="21" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D391" s="1" t="n">
         <v>8</v>
@@ -19424,7 +19430,7 @@
         <v>34.25</v>
       </c>
       <c r="N391" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O391" s="38" t="n">
         <v>5</v>
@@ -19438,10 +19444,10 @@
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B392" s="21" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C392" s="21" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D392" s="1" t="n">
         <v>8</v>
@@ -19476,7 +19482,7 @@
         <v>34.5</v>
       </c>
       <c r="N392" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O392" s="38" t="n">
         <v>5</v>
@@ -19493,7 +19499,7 @@
         <v>545</v>
       </c>
       <c r="C393" s="21" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D393" s="1" t="n">
         <v>8</v>
@@ -19528,7 +19534,7 @@
         <v>34.75</v>
       </c>
       <c r="N393" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O393" s="38" t="n">
         <v>5</v>
@@ -19542,10 +19548,10 @@
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B394" s="3" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C394" s="3" t="s">
-        <v>465</v>
+        <v>627</v>
       </c>
       <c r="D394" s="1" t="n">
         <v>16</v>
@@ -19605,7 +19611,7 @@
         <v>16</v>
       </c>
       <c r="E395" s="33" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F395" s="33"/>
       <c r="G395" s="33" t="n">
@@ -19723,22 +19729,22 @@
     <row r="6" s="43" customFormat="true" ht="34.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="44"/>
       <c r="C6" s="44" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="F6" s="44" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="G6" s="44" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="I6" s="44"/>
     </row>

</xml_diff>

<commit_message>
Fix the payload lengths in the frame descriptions.  The only payload change here is adding the conversion for the DCT RSSI
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecGolf-T.xlsx
+++ b/genSpacecraft/DownlinkSpecGolf-T.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="651">
   <si>
     <t xml:space="preserve">//</t>
   </si>
@@ -404,7 +404,10 @@
     <t xml:space="preserve">DCT1RSSI</t>
   </si>
   <si>
-    <t xml:space="preserve">-dBm</t>
+    <t xml:space="preserve">dct_rssi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dBm</t>
   </si>
   <si>
     <t xml:space="preserve">DCT1 RSSI</t>
@@ -413,7 +416,7 @@
     <t xml:space="preserve">Secndry RSSI</t>
   </si>
   <si>
-    <t xml:space="preserve">DCT2RSSO</t>
+    <t xml:space="preserve">DCT2RSSI</t>
   </si>
   <si>
     <t xml:space="preserve">DCT2 RSSI</t>
@@ -489,9 +492,6 @@
   </si>
   <si>
     <t xml:space="preserve">RSSI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dBm</t>
   </si>
   <si>
     <t xml:space="preserve">Received Signal Strength Indication</t>
@@ -2323,8 +2323,8 @@
   </sheetPr>
   <dimension ref="A1:Q405"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q87" activeCellId="0" sqref="Q87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G53" activeCellId="0" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4223,14 +4223,14 @@
         <v>26</v>
       </c>
       <c r="F49" s="22"/>
-      <c r="G49" s="22" t="n">
-        <v>1</v>
+      <c r="G49" s="22" t="s">
+        <v>127</v>
       </c>
       <c r="H49" s="21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I49" s="22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J49" s="26" t="n">
         <f aca="false">J48+D48</f>
@@ -4263,10 +4263,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="28" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D50" s="28" t="n">
         <v>8</v>
@@ -4275,14 +4275,14 @@
         <v>26</v>
       </c>
       <c r="F50" s="22"/>
-      <c r="G50" s="22" t="n">
-        <v>1</v>
+      <c r="G50" s="22" t="s">
+        <v>127</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I50" s="22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J50" s="26" t="n">
         <f aca="false">J49+D49</f>
@@ -4315,10 +4315,10 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D51" s="28" t="n">
         <v>8</v>
@@ -4367,10 +4367,10 @@
     </row>
     <row r="52" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D52" s="28" t="n">
         <v>8</v>
@@ -4384,7 +4384,7 @@
       </c>
       <c r="H52" s="21"/>
       <c r="I52" s="28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J52" s="26" t="n">
         <f aca="false">J51+D51</f>
@@ -4417,10 +4417,10 @@
     </row>
     <row r="53" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D53" s="28" t="n">
         <v>8</v>
@@ -4430,13 +4430,13 @@
       </c>
       <c r="F53" s="22"/>
       <c r="G53" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>74</v>
       </c>
       <c r="I53" s="28" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J53" s="26" t="n">
         <f aca="false">J52+D52</f>
@@ -4455,7 +4455,7 @@
         <v>4.75</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O53" s="1" t="n">
         <v>6</v>
@@ -4469,10 +4469,10 @@
     </row>
     <row r="54" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D54" s="28" t="n">
         <v>8</v>
@@ -4482,13 +4482,13 @@
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I54" s="22" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J54" s="26" t="n">
         <f aca="false">J53+D53</f>
@@ -4521,10 +4521,10 @@
     </row>
     <row r="55" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="28" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D55" s="28" t="n">
         <v>8</v>
@@ -4540,7 +4540,7 @@
         <v>83</v>
       </c>
       <c r="I55" s="22" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J55" s="26" t="n">
         <f aca="false">J54+D54</f>
@@ -4573,10 +4573,10 @@
     </row>
     <row r="56" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D56" s="28" t="n">
         <v>8</v>
@@ -4592,7 +4592,7 @@
         <v>68</v>
       </c>
       <c r="I56" s="22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J56" s="26" t="n">
         <f aca="false">J55+D55</f>
@@ -4625,10 +4625,10 @@
     </row>
     <row r="57" customFormat="false" ht="50.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="28" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D57" s="28" t="n">
         <v>8</v>
@@ -4638,10 +4638,10 @@
       </c>
       <c r="F57" s="22"/>
       <c r="G57" s="22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="I57" s="22" t="s">
         <v>157</v>
@@ -4715,7 +4715,7 @@
         <v>6</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O58" s="1" t="n">
         <v>6</v>
@@ -4767,7 +4767,7 @@
         <v>6.25</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O59" s="1" t="n">
         <v>6</v>
@@ -4819,7 +4819,7 @@
         <v>6.5</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O60" s="1" t="n">
         <v>6</v>
@@ -4871,7 +4871,7 @@
         <v>6.75</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O61" s="1" t="n">
         <v>6</v>
@@ -4923,7 +4923,7 @@
         <v>7</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O62" s="1" t="n">
         <v>6</v>
@@ -4975,7 +4975,7 @@
         <v>7.25</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O63" s="1" t="n">
         <v>6</v>
@@ -5027,7 +5027,7 @@
         <v>7.5</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O64" s="1" t="n">
         <v>6</v>
@@ -5079,7 +5079,7 @@
         <v>7.75</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O65" s="1" t="n">
         <v>6</v>
@@ -6146,13 +6146,13 @@
       </c>
       <c r="F86" s="22"/>
       <c r="G86" s="22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I86" s="22" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J86" s="26" t="n">
         <f aca="false">J85+D85</f>
@@ -6685,7 +6685,7 @@
         <v>14.625</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O99" s="1" t="n">
         <v>6</v>
@@ -9487,7 +9487,7 @@
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C164" s="28" t="s">
         <v>371</v>
@@ -9836,7 +9836,7 @@
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B174" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C174" s="28" t="s">
         <v>385</v>
@@ -9886,7 +9886,7 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B175" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C175" s="28" t="s">
         <v>386</v>
@@ -20179,7 +20179,7 @@
       <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.11"/>

</xml_diff>

<commit_message>
Change conversions for MESAT and use a new design for "invalid" values
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecGolf-T.xlsx
+++ b/genSpacecraft/DownlinkSpecGolf-T.xlsx
@@ -941,7 +941,7 @@
     <t xml:space="preserve">wodSize</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of WOD data payloads kept for each of Science and Housekeeping.  In hundreds</t>
+    <t xml:space="preserve">Number of WOD data payloads kept for each of Science and Housekeeping</t>
   </si>
   <si>
     <t xml:space="preserve">Diagnostic</t>
@@ -2523,8 +2523,8 @@
   </sheetPr>
   <dimension ref="A1:Q425"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A248" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G268" activeCellId="0" sqref="G268"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A184" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I184" activeCellId="0" sqref="I184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8040,7 +8040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="30" t="s">
         <v>304</v>
       </c>
@@ -21294,7 +21294,7 @@
       <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.11"/>

</xml_diff>